<commit_message>
Sprint and Product backlog updates
</commit_message>
<xml_diff>
--- a/documents/FlyingMongeese_Deliverable_2_SprintBacklog.xlsx
+++ b/documents/FlyingMongeese_Deliverable_2_SprintBacklog.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cadew\OneDrive\Documents\GitHub\Software2project\documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB5CB1EC-FA99-4147-AB67-A1E85ED0C23B}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{88F9F640-2C47-47C4-9DF5-8D73302B79BF}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="435" windowWidth="22740" windowHeight="15555" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="333" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="355" uniqueCount="69">
   <si>
     <t>User Story</t>
   </si>
@@ -239,6 +239,45 @@
   </si>
   <si>
     <t>Week 2 (2/05/2018)</t>
+  </si>
+  <si>
+    <t>Cade:X
+Andre:
+Turner:
+Mayur:
+Riggs:
+Carolyn:</t>
+  </si>
+  <si>
+    <t>Meet with people for focus group</t>
+  </si>
+  <si>
+    <t>Cade:X
+Andre:X
+Turner:
+Mayur:
+Riggs:
+Carolyn:</t>
+  </si>
+  <si>
+    <t>Sprint Backlog</t>
+  </si>
+  <si>
+    <t>Fix document</t>
+  </si>
+  <si>
+    <t>Update document</t>
+  </si>
+  <si>
+    <t>Finalize document
+Meet with focus group</t>
+  </si>
+  <si>
+    <t>Create and fill out document</t>
+  </si>
+  <si>
+    <t>Create and fill the document 
+Update the document</t>
   </si>
 </sst>
 </file>
@@ -690,8 +729,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+    <sheetView tabSelected="1" topLeftCell="A14" workbookViewId="0">
+      <selection activeCell="E20" sqref="E20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -778,7 +817,7 @@
       <c r="J3" s="6"/>
       <c r="K3" s="6"/>
     </row>
-    <row r="4" spans="1:11" ht="102" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:11" ht="89.25" x14ac:dyDescent="0.2">
       <c r="A4" s="11">
         <v>12</v>
       </c>
@@ -824,7 +863,7 @@
       <c r="J5" s="6"/>
       <c r="K5" s="6"/>
     </row>
-    <row r="6" spans="1:11" ht="89.25" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:11" ht="76.5" x14ac:dyDescent="0.2">
       <c r="A6" s="11">
         <v>14</v>
       </c>
@@ -847,7 +886,7 @@
       <c r="J6" s="6"/>
       <c r="K6" s="6"/>
     </row>
-    <row r="7" spans="1:11" ht="89.25" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:11" ht="76.5" x14ac:dyDescent="0.2">
       <c r="A7" s="11">
         <v>15</v>
       </c>
@@ -1011,7 +1050,9 @@
       </c>
       <c r="C14" s="8"/>
       <c r="D14" s="8"/>
-      <c r="E14" s="8"/>
+      <c r="E14" s="8" t="s">
+        <v>67</v>
+      </c>
       <c r="F14" s="13" t="s">
         <v>10</v>
       </c>
@@ -1026,12 +1067,14 @@
       </c>
       <c r="C15" s="8"/>
       <c r="D15" s="8"/>
-      <c r="E15" s="8"/>
+      <c r="E15" s="8" t="s">
+        <v>67</v>
+      </c>
       <c r="F15" s="13" t="s">
-        <v>10</v>
+        <v>60</v>
       </c>
       <c r="G15" s="13" t="s">
-        <v>10</v>
+        <v>60</v>
       </c>
     </row>
     <row r="16" spans="1:11" ht="76.5" x14ac:dyDescent="0.2">
@@ -1041,7 +1084,9 @@
       </c>
       <c r="C16" s="8"/>
       <c r="D16" s="8"/>
-      <c r="E16" s="8"/>
+      <c r="E16" s="8" t="s">
+        <v>67</v>
+      </c>
       <c r="F16" s="13" t="s">
         <v>10</v>
       </c>
@@ -1056,12 +1101,14 @@
       </c>
       <c r="C17" s="8"/>
       <c r="D17" s="8"/>
-      <c r="E17" s="8"/>
+      <c r="E17" s="8" t="s">
+        <v>67</v>
+      </c>
       <c r="F17" s="13" t="s">
-        <v>10</v>
+        <v>60</v>
       </c>
       <c r="G17" s="13" t="s">
-        <v>10</v>
+        <v>60</v>
       </c>
     </row>
     <row r="18" spans="1:7" ht="76.5" x14ac:dyDescent="0.2">
@@ -1071,12 +1118,14 @@
       </c>
       <c r="C18" s="8"/>
       <c r="D18" s="8"/>
-      <c r="E18" s="8"/>
+      <c r="E18" s="8" t="s">
+        <v>67</v>
+      </c>
       <c r="F18" s="13" t="s">
-        <v>10</v>
+        <v>60</v>
       </c>
       <c r="G18" s="13" t="s">
-        <v>10</v>
+        <v>60</v>
       </c>
     </row>
     <row r="19" spans="1:7" ht="76.5" x14ac:dyDescent="0.2">
@@ -1086,16 +1135,29 @@
       </c>
       <c r="C19" s="8"/>
       <c r="D19" s="8"/>
-      <c r="E19" s="8"/>
+      <c r="E19" s="8" t="s">
+        <v>67</v>
+      </c>
       <c r="F19" s="13" t="s">
-        <v>10</v>
+        <v>60</v>
       </c>
       <c r="G19" s="13" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="B20" s="7"/>
+        <v>60</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" ht="76.5" x14ac:dyDescent="0.2">
+      <c r="B20" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="E20" s="14" t="s">
+        <v>68</v>
+      </c>
+      <c r="F20" s="13" t="s">
+        <v>60</v>
+      </c>
+      <c r="G20" s="13" t="s">
+        <v>60</v>
+      </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B21" s="7"/>
@@ -1117,8 +1179,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:K21"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="E5" sqref="A1:G21"/>
+    <sheetView topLeftCell="A11" workbookViewId="0">
+      <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1443,7 +1505,9 @@
       </c>
       <c r="C15" s="15"/>
       <c r="D15" s="15"/>
-      <c r="E15" s="15"/>
+      <c r="E15" s="8" t="s">
+        <v>67</v>
+      </c>
       <c r="F15" s="18" t="s">
         <v>10</v>
       </c>
@@ -1473,9 +1537,11 @@
       </c>
       <c r="C17" s="15"/>
       <c r="D17" s="15"/>
-      <c r="E17" s="15"/>
+      <c r="E17" s="19" t="s">
+        <v>61</v>
+      </c>
       <c r="F17" s="18" t="s">
-        <v>10</v>
+        <v>62</v>
       </c>
       <c r="G17" s="18" t="s">
         <v>10</v>
@@ -1533,12 +1599,14 @@
       </c>
       <c r="C21" s="15"/>
       <c r="D21" s="15"/>
-      <c r="E21" s="15"/>
+      <c r="E21" s="15" t="s">
+        <v>65</v>
+      </c>
       <c r="F21" s="18" t="s">
-        <v>10</v>
+        <v>60</v>
       </c>
       <c r="G21" s="18" t="s">
-        <v>10</v>
+        <v>60</v>
       </c>
     </row>
   </sheetData>
@@ -1555,8 +1623,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B2B9D4EE-EF66-4647-A07F-23214E7A01E8}">
   <dimension ref="A1:G24"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:G22"/>
+    <sheetView topLeftCell="A15" workbookViewId="0">
+      <selection activeCell="E23" sqref="E23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1564,7 +1632,7 @@
     <col min="2" max="2" width="28.7109375" customWidth="1"/>
     <col min="3" max="3" width="10" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="11.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="6" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.85546875" bestFit="1" customWidth="1"/>
     <col min="6" max="7" width="10.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1818,9 +1886,11 @@
       </c>
       <c r="C14" s="8"/>
       <c r="D14" s="8"/>
-      <c r="E14" s="8"/>
+      <c r="E14" s="8" t="s">
+        <v>64</v>
+      </c>
       <c r="F14" s="13" t="s">
-        <v>10</v>
+        <v>60</v>
       </c>
       <c r="G14" s="13" t="s">
         <v>10</v>
@@ -1833,9 +1903,11 @@
       </c>
       <c r="C15" s="8"/>
       <c r="D15" s="8"/>
-      <c r="E15" s="8"/>
+      <c r="E15" s="8" t="s">
+        <v>64</v>
+      </c>
       <c r="F15" s="13" t="s">
-        <v>10</v>
+        <v>60</v>
       </c>
       <c r="G15" s="13" t="s">
         <v>10</v>
@@ -1848,9 +1920,11 @@
       </c>
       <c r="C16" s="8"/>
       <c r="D16" s="8"/>
-      <c r="E16" s="8"/>
+      <c r="E16" s="8" t="s">
+        <v>67</v>
+      </c>
       <c r="F16" s="13" t="s">
-        <v>10</v>
+        <v>60</v>
       </c>
       <c r="G16" s="13" t="s">
         <v>10</v>
@@ -1863,9 +1937,11 @@
       </c>
       <c r="C17" s="8"/>
       <c r="D17" s="8"/>
-      <c r="E17" s="8"/>
+      <c r="E17" s="8" t="s">
+        <v>64</v>
+      </c>
       <c r="F17" s="13" t="s">
-        <v>10</v>
+        <v>60</v>
       </c>
       <c r="G17" s="13" t="s">
         <v>10</v>
@@ -1878,9 +1954,11 @@
       </c>
       <c r="C18" s="8"/>
       <c r="D18" s="8"/>
-      <c r="E18" s="8"/>
+      <c r="E18" s="14" t="s">
+        <v>66</v>
+      </c>
       <c r="F18" s="13" t="s">
-        <v>10</v>
+        <v>60</v>
       </c>
       <c r="G18" s="13" t="s">
         <v>10</v>
@@ -1893,7 +1971,9 @@
       </c>
       <c r="C19" s="8"/>
       <c r="D19" s="8"/>
-      <c r="E19" s="8"/>
+      <c r="E19" s="8" t="s">
+        <v>67</v>
+      </c>
       <c r="F19" s="13" t="s">
         <v>10</v>
       </c>
@@ -1908,7 +1988,9 @@
       </c>
       <c r="C20" s="8"/>
       <c r="D20" s="8"/>
-      <c r="E20" s="8"/>
+      <c r="E20" s="8" t="s">
+        <v>67</v>
+      </c>
       <c r="F20" s="13" t="s">
         <v>10</v>
       </c>
@@ -1923,7 +2005,9 @@
       </c>
       <c r="C21" s="8"/>
       <c r="D21" s="8"/>
-      <c r="E21" s="8"/>
+      <c r="E21" s="8" t="s">
+        <v>67</v>
+      </c>
       <c r="F21" s="13" t="s">
         <v>10</v>
       </c>
@@ -1938,7 +2022,9 @@
       </c>
       <c r="C22" s="8"/>
       <c r="D22" s="8"/>
-      <c r="E22" s="8"/>
+      <c r="E22" s="8" t="s">
+        <v>65</v>
+      </c>
       <c r="F22" s="13" t="s">
         <v>10</v>
       </c>

</xml_diff>